<commit_message>
Update job postings for 2024-12-01
</commit_message>
<xml_diff>
--- a/javascript-jobs-post/12-1-2024_post.xlsx
+++ b/javascript-jobs-post/12-1-2024_post.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="317" count="317">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="316" count="316">
   <x:si>
     <x:t>companyPhoto</x:t>
   </x:si>
@@ -52,7 +52,7 @@
     <x:t>Tether Operations Limited</x:t>
   </x:si>
   <x:si>
-    <x:t>1D</x:t>
+    <x:t>2D</x:t>
   </x:si>
   <x:si>
     <x:t/>
@@ -118,9 +118,6 @@
     <x:t>Sr Backend Developer Node JS + AI (100% remote - Switzerland)</x:t>
   </x:si>
   <x:si>
-    <x:t>2D</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://javascript.jobs/job/sr-backend-developer-node-js-ai-100-remote-france</x:t>
   </x:si>
   <x:si>
@@ -205,6 +202,9 @@
     <x:t>Sr Backend Developer Node JS + AI (100% remote - Ireland)</x:t>
   </x:si>
   <x:si>
+    <x:t>3D</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/storage/images/company/6714ee3d0b783.jpg</x:t>
   </x:si>
   <x:si>
@@ -292,9 +292,6 @@
     <x:t>Halo Media</x:t>
   </x:si>
   <x:si>
-    <x:t>3D</x:t>
-  </x:si>
-  <x:si>
     <x:t>India</x:t>
   </x:si>
   <x:si>
@@ -385,6 +382,9 @@
     <x:t>Sr Backend Developer Node JS + AI (100% remote - Germany)</x:t>
   </x:si>
   <x:si>
+    <x:t>4D</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/job/sr-backend-developer-node-js-ai-100-remote-colombia</x:t>
   </x:si>
   <x:si>
@@ -499,9 +499,6 @@
     <x:t>Deel</x:t>
   </x:si>
   <x:si>
-    <x:t>4D</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://javascript.jobs/job/senior-backend-developer-node-100-remote-colombia</x:t>
   </x:si>
   <x:si>
@@ -604,6 +601,9 @@
     <x:t>Factor Eleven</x:t>
   </x:si>
   <x:si>
+    <x:t>5D</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/job/technical-lead-react-native-4</x:t>
   </x:si>
   <x:si>
@@ -622,9 +622,6 @@
     <x:t>Leidos</x:t>
   </x:si>
   <x:si>
-    <x:t>5D</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://javascript.jobs/job/senior-backend-developer-node-100-remote-poland</x:t>
   </x:si>
   <x:si>
@@ -658,6 +655,9 @@
     <x:t>DaCodes</x:t>
   </x:si>
   <x:si>
+    <x:t>6D</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/job/senior-software-engineer-typescript-4</x:t>
   </x:si>
   <x:si>
@@ -700,9 +700,6 @@
     <x:t>Engineering Manager (JavaScript / NodeJS / Typescript) (Spain, Remote, f/m/d)</x:t>
   </x:si>
   <x:si>
-    <x:t>6D</x:t>
-  </x:si>
-  <x:si>
     <x:t>https://javascript.jobs/storage/images/company/6714ed84739bc.png</x:t>
   </x:si>
   <x:si>
@@ -727,6 +724,9 @@
     <x:t>Phoenix Cyber</x:t>
   </x:si>
   <x:si>
+    <x:t>1W</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://javascript.jobs/job/technical-lead-react-native-3</x:t>
   </x:si>
   <x:si>
@@ -767,9 +767,6 @@
   </x:si>
   <x:si>
     <x:t>AlgaeCal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1W</x:t>
   </x:si>
   <x:si>
     <x:t>Philippines</x:t>
@@ -1574,7 +1571,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
         <x:v>13</x:v>
@@ -1585,10 +1582,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
         <x:v>35</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>36</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>10</x:v>
@@ -1597,7 +1594,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
         <x:v>13</x:v>
@@ -1608,10 +1605,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
         <x:v>37</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>38</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>10</x:v>
@@ -1620,7 +1617,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
         <x:v>13</x:v>
@@ -1631,10 +1628,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
         <x:v>39</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>40</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>10</x:v>
@@ -1643,7 +1640,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
         <x:v>13</x:v>
@@ -1654,10 +1651,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
         <x:v>41</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>42</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>10</x:v>
@@ -1666,7 +1663,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
         <x:v>13</x:v>
@@ -1674,25 +1671,25 @@
     </x:row>
     <x:row r="16" spans="1:7">
       <x:c r="A16" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="B16" s="0" t="s">
+      <x:c r="C16" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C16" s="0" t="s">
+      <x:c r="D16" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
+      <x:c r="F16" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="F16" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="G16" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
@@ -1700,10 +1697,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>48</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>49</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>10</x:v>
@@ -1712,7 +1709,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
         <x:v>13</x:v>
@@ -1720,25 +1717,25 @@
     </x:row>
     <x:row r="18" spans="1:7">
       <x:c r="A18" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="B18" s="0" t="s">
+      <x:c r="C18" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="C18" s="0" t="s">
+      <x:c r="D18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
+      <x:c r="F18" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="G18" s="0" t="s">
-        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:7">
@@ -1746,10 +1743,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
         <x:v>55</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>56</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>10</x:v>
@@ -1758,7 +1755,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
         <x:v>13</x:v>
@@ -1769,10 +1766,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
         <x:v>57</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>58</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>10</x:v>
@@ -1781,7 +1778,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
         <x:v>13</x:v>
@@ -1792,10 +1789,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
         <x:v>59</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>60</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>10</x:v>
@@ -1804,7 +1801,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
         <x:v>13</x:v>
@@ -1815,10 +1812,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
         <x:v>61</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>62</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
         <x:v>10</x:v>
@@ -1827,7 +1824,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
         <x:v>13</x:v>
@@ -1850,7 +1847,7 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
         <x:v>67</x:v>
@@ -1873,7 +1870,7 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
         <x:v>13</x:v>
@@ -1896,7 +1893,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
         <x:v>13</x:v>
@@ -1919,7 +1916,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
         <x:v>13</x:v>
@@ -1942,7 +1939,7 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
         <x:v>13</x:v>
@@ -1965,7 +1962,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
         <x:v>13</x:v>
@@ -1988,7 +1985,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
         <x:v>13</x:v>
@@ -2011,7 +2008,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
         <x:v>13</x:v>
@@ -2034,7 +2031,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
         <x:v>13</x:v>
@@ -2057,7 +2054,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
         <x:v>13</x:v>
@@ -2080,10 +2077,10 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="F33" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="G33" s="0" t="s">
         <x:v>92</x:v>
-      </x:c>
-      <x:c r="G33" s="0" t="s">
-        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:7">
@@ -2091,10 +2088,10 @@
         <x:v>74</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
         <x:v>94</x:v>
-      </x:c>
-      <x:c r="C34" s="0" t="s">
-        <x:v>95</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
         <x:v>10</x:v>
@@ -2103,7 +2100,7 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="F34" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G34" s="0" t="s">
         <x:v>13</x:v>
@@ -2111,25 +2108,25 @@
     </x:row>
     <x:row r="35" spans="1:7">
       <x:c r="A35" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
         <x:v>96</x:v>
       </x:c>
-      <x:c r="B35" s="0" t="s">
+      <x:c r="C35" s="0" t="s">
         <x:v>97</x:v>
       </x:c>
-      <x:c r="C35" s="0" t="s">
+      <x:c r="D35" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="D35" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E35" s="0" t="s">
-        <x:v>99</x:v>
-      </x:c>
       <x:c r="F35" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G35" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:7">
@@ -2137,10 +2134,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
         <x:v>100</x:v>
-      </x:c>
-      <x:c r="C36" s="0" t="s">
-        <x:v>101</x:v>
       </x:c>
       <x:c r="D36" s="0" t="s">
         <x:v>10</x:v>
@@ -2149,7 +2146,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F36" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
         <x:v>13</x:v>
@@ -2160,10 +2157,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
         <x:v>102</x:v>
-      </x:c>
-      <x:c r="C37" s="0" t="s">
-        <x:v>103</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
         <x:v>10</x:v>
@@ -2172,7 +2169,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G37" s="0" t="s">
         <x:v>13</x:v>
@@ -2180,48 +2177,48 @@
     </x:row>
     <x:row r="38" spans="1:7">
       <x:c r="A38" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
         <x:v>104</x:v>
       </x:c>
-      <x:c r="B38" s="0" t="s">
+      <x:c r="C38" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
-      <x:c r="C38" s="0" t="s">
+      <x:c r="D38" s="0" t="s">
         <x:v>106</x:v>
       </x:c>
-      <x:c r="D38" s="0" t="s">
+      <x:c r="E38" s="0" t="s">
         <x:v>107</x:v>
       </x:c>
-      <x:c r="E38" s="0" t="s">
+      <x:c r="F38" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="G38" s="0" t="s">
         <x:v>108</x:v>
-      </x:c>
-      <x:c r="F38" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="G38" s="0" t="s">
-        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:7">
       <x:c r="A39" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
         <x:v>110</x:v>
       </x:c>
-      <x:c r="B39" s="0" t="s">
+      <x:c r="C39" s="0" t="s">
         <x:v>111</x:v>
       </x:c>
-      <x:c r="C39" s="0" t="s">
+      <x:c r="D39" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
         <x:v>112</x:v>
       </x:c>
-      <x:c r="D39" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E39" s="0" t="s">
-        <x:v>113</x:v>
-      </x:c>
       <x:c r="F39" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="G39" s="0" t="s">
         <x:v>92</x:v>
-      </x:c>
-      <x:c r="G39" s="0" t="s">
-        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:7">
@@ -2229,10 +2226,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
         <x:v>114</x:v>
-      </x:c>
-      <x:c r="C40" s="0" t="s">
-        <x:v>115</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
         <x:v>10</x:v>
@@ -2241,7 +2238,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
         <x:v>13</x:v>
@@ -2249,25 +2246,25 @@
     </x:row>
     <x:row r="41" spans="1:7">
       <x:c r="A41" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
         <x:v>116</x:v>
       </x:c>
-      <x:c r="B41" s="0" t="s">
+      <x:c r="C41" s="0" t="s">
         <x:v>117</x:v>
       </x:c>
-      <x:c r="C41" s="0" t="s">
+      <x:c r="D41" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
         <x:v>118</x:v>
       </x:c>
-      <x:c r="D41" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E41" s="0" t="s">
+      <x:c r="F41" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="G41" s="0" t="s">
         <x:v>119</x:v>
-      </x:c>
-      <x:c r="F41" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="G41" s="0" t="s">
-        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:7">
@@ -2275,10 +2272,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
         <x:v>121</x:v>
-      </x:c>
-      <x:c r="C42" s="0" t="s">
-        <x:v>122</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
         <x:v>10</x:v>
@@ -2287,7 +2284,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F42" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
         <x:v>13</x:v>
@@ -2310,7 +2307,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
         <x:v>13</x:v>
@@ -2333,7 +2330,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F44" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G44" s="0" t="s">
         <x:v>13</x:v>
@@ -2356,7 +2353,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F45" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G45" s="0" t="s">
         <x:v>13</x:v>
@@ -2379,7 +2376,7 @@
         <x:v>132</x:v>
       </x:c>
       <x:c r="F46" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G46" s="0" t="s">
         <x:v>133</x:v>
@@ -2402,7 +2399,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G47" s="0" t="s">
         <x:v>13</x:v>
@@ -2410,25 +2407,25 @@
     </x:row>
     <x:row r="48" spans="1:7">
       <x:c r="A48" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
         <x:v>136</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="D48" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E48" s="0" t="s">
+      <x:c r="F48" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="G48" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="F48" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="G48" s="0" t="s">
-        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:7">
@@ -2448,7 +2445,7 @@
         <x:v>140</x:v>
       </x:c>
       <x:c r="F49" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G49" s="0" t="s">
         <x:v>141</x:v>
@@ -2471,7 +2468,7 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="F50" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G50" s="0" t="s">
         <x:v>146</x:v>
@@ -2494,7 +2491,7 @@
         <x:v>150</x:v>
       </x:c>
       <x:c r="F51" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G51" s="0" t="s">
         <x:v>151</x:v>
@@ -2517,7 +2514,7 @@
         <x:v>155</x:v>
       </x:c>
       <x:c r="F52" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G52" s="0" t="s">
         <x:v>156</x:v>
@@ -2540,7 +2537,7 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="F53" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G53" s="0" t="s">
         <x:v>13</x:v>
@@ -2551,10 +2548,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
         <x:v>162</x:v>
-      </x:c>
-      <x:c r="C54" s="0" t="s">
-        <x:v>163</x:v>
       </x:c>
       <x:c r="D54" s="0" t="s">
         <x:v>10</x:v>
@@ -2563,7 +2560,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F54" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G54" s="0" t="s">
         <x:v>13</x:v>
@@ -2574,10 +2571,10 @@
         <x:v>142</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
         <x:v>164</x:v>
-      </x:c>
-      <x:c r="C55" s="0" t="s">
-        <x:v>165</x:v>
       </x:c>
       <x:c r="D55" s="0" t="s">
         <x:v>10</x:v>
@@ -2586,53 +2583,53 @@
         <x:v>145</x:v>
       </x:c>
       <x:c r="F55" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G55" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>165</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:7">
       <x:c r="A56" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
         <x:v>167</x:v>
       </x:c>
-      <x:c r="B56" s="0" t="s">
+      <x:c r="C56" s="0" t="s">
         <x:v>168</x:v>
       </x:c>
-      <x:c r="C56" s="0" t="s">
+      <x:c r="D56" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E56" s="0" t="s">
         <x:v>169</x:v>
       </x:c>
-      <x:c r="D56" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E56" s="0" t="s">
-        <x:v>170</x:v>
-      </x:c>
       <x:c r="F56" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G56" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:7">
       <x:c r="A57" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
         <x:v>171</x:v>
       </x:c>
-      <x:c r="B57" s="0" t="s">
+      <x:c r="C57" s="0" t="s">
         <x:v>172</x:v>
       </x:c>
-      <x:c r="C57" s="0" t="s">
+      <x:c r="D57" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E57" s="0" t="s">
         <x:v>173</x:v>
       </x:c>
-      <x:c r="D57" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E57" s="0" t="s">
-        <x:v>174</x:v>
-      </x:c>
       <x:c r="F57" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G57" s="0" t="s">
         <x:v>151</x:v>
@@ -2640,45 +2637,45 @@
     </x:row>
     <x:row r="58" spans="1:7">
       <x:c r="A58" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
         <x:v>175</x:v>
       </x:c>
-      <x:c r="B58" s="0" t="s">
+      <x:c r="C58" s="0" t="s">
         <x:v>176</x:v>
       </x:c>
-      <x:c r="C58" s="0" t="s">
+      <x:c r="D58" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E58" s="0" t="s">
         <x:v>177</x:v>
       </x:c>
-      <x:c r="D58" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E58" s="0" t="s">
-        <x:v>178</x:v>
-      </x:c>
       <x:c r="F58" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G58" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:7">
       <x:c r="A59" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
         <x:v>179</x:v>
       </x:c>
-      <x:c r="B59" s="0" t="s">
+      <x:c r="C59" s="0" t="s">
         <x:v>180</x:v>
       </x:c>
-      <x:c r="C59" s="0" t="s">
+      <x:c r="D59" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E59" s="0" t="s">
         <x:v>181</x:v>
       </x:c>
-      <x:c r="D59" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E59" s="0" t="s">
-        <x:v>182</x:v>
-      </x:c>
       <x:c r="F59" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G59" s="0" t="s">
         <x:v>13</x:v>
@@ -2686,22 +2683,22 @@
     </x:row>
     <x:row r="60" spans="1:7">
       <x:c r="A60" s="0" t="s">
+        <x:v>182</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
         <x:v>183</x:v>
       </x:c>
-      <x:c r="B60" s="0" t="s">
+      <x:c r="C60" s="0" t="s">
         <x:v>184</x:v>
       </x:c>
-      <x:c r="C60" s="0" t="s">
+      <x:c r="D60" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E60" s="0" t="s">
         <x:v>185</x:v>
       </x:c>
-      <x:c r="D60" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E60" s="0" t="s">
-        <x:v>186</x:v>
-      </x:c>
       <x:c r="F60" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="G60" s="0" t="s">
         <x:v>13</x:v>
@@ -2709,68 +2706,68 @@
     </x:row>
     <x:row r="61" spans="1:7">
       <x:c r="A61" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
         <x:v>187</x:v>
       </x:c>
-      <x:c r="B61" s="0" t="s">
+      <x:c r="C61" s="0" t="s">
         <x:v>188</x:v>
       </x:c>
-      <x:c r="C61" s="0" t="s">
+      <x:c r="D61" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E61" s="0" t="s">
         <x:v>189</x:v>
       </x:c>
-      <x:c r="D61" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E61" s="0" t="s">
+      <x:c r="F61" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="G61" s="0" t="s">
         <x:v>190</x:v>
-      </x:c>
-      <x:c r="F61" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
-      <x:c r="G61" s="0" t="s">
-        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:7">
       <x:c r="A62" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
         <x:v>192</x:v>
       </x:c>
-      <x:c r="B62" s="0" t="s">
+      <x:c r="C62" s="0" t="s">
         <x:v>193</x:v>
       </x:c>
-      <x:c r="C62" s="0" t="s">
+      <x:c r="D62" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E62" s="0" t="s">
         <x:v>194</x:v>
       </x:c>
-      <x:c r="D62" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E62" s="0" t="s">
+      <x:c r="F62" s="0" t="s">
         <x:v>195</x:v>
       </x:c>
-      <x:c r="F62" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
       <x:c r="G62" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:7">
       <x:c r="A63" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
         <x:v>196</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E63" s="0" t="s">
         <x:v>189</x:v>
       </x:c>
-      <x:c r="D63" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E63" s="0" t="s">
-        <x:v>190</x:v>
-      </x:c>
       <x:c r="F63" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="G63" s="0" t="s">
         <x:v>197</x:v>
@@ -2793,7 +2790,7 @@
         <x:v>201</x:v>
       </x:c>
       <x:c r="F64" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="G64" s="0" t="s">
         <x:v>133</x:v>
@@ -2804,10 +2801,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
         <x:v>203</x:v>
-      </x:c>
-      <x:c r="C65" s="0" t="s">
-        <x:v>204</x:v>
       </x:c>
       <x:c r="D65" s="0" t="s">
         <x:v>10</x:v>
@@ -2816,7 +2813,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F65" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="G65" s="0" t="s">
         <x:v>133</x:v>
@@ -2824,53 +2821,53 @@
     </x:row>
     <x:row r="66" spans="1:7">
       <x:c r="A66" s="0" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
         <x:v>205</x:v>
       </x:c>
-      <x:c r="B66" s="0" t="s">
+      <x:c r="C66" s="0" t="s">
         <x:v>206</x:v>
       </x:c>
-      <x:c r="C66" s="0" t="s">
+      <x:c r="D66" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E66" s="0" t="s">
         <x:v>207</x:v>
       </x:c>
-      <x:c r="D66" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E66" s="0" t="s">
+      <x:c r="F66" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="G66" s="0" t="s">
         <x:v>208</x:v>
-      </x:c>
-      <x:c r="F66" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
-      <x:c r="G66" s="0" t="s">
-        <x:v>209</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:7">
       <x:c r="A67" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
         <x:v>210</x:v>
       </x:c>
-      <x:c r="B67" s="0" t="s">
+      <x:c r="C67" s="0" t="s">
         <x:v>211</x:v>
       </x:c>
-      <x:c r="C67" s="0" t="s">
+      <x:c r="D67" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E67" s="0" t="s">
         <x:v>212</x:v>
       </x:c>
-      <x:c r="D67" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E67" s="0" t="s">
+      <x:c r="F67" s="0" t="s">
         <x:v>213</x:v>
       </x:c>
-      <x:c r="F67" s="0" t="s">
-        <x:v>202</x:v>
-      </x:c>
       <x:c r="G67" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:7">
       <x:c r="A68" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
         <x:v>214</x:v>
@@ -2882,13 +2879,13 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="E68" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F68" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G68" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:7">
@@ -2908,7 +2905,7 @@
         <x:v>219</x:v>
       </x:c>
       <x:c r="F69" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G69" s="0" t="s">
         <x:v>13</x:v>
@@ -2931,7 +2928,7 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="F70" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G70" s="0" t="s">
         <x:v>13</x:v>
@@ -2954,7 +2951,7 @@
         <x:v>225</x:v>
       </x:c>
       <x:c r="F71" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G71" s="0" t="s">
         <x:v>13</x:v>
@@ -2962,7 +2959,7 @@
     </x:row>
     <x:row r="72" spans="1:7">
       <x:c r="A72" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
         <x:v>226</x:v>
@@ -2974,10 +2971,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="E72" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="F72" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G72" s="0" t="s">
         <x:v>141</x:v>
@@ -2985,22 +2982,22 @@
     </x:row>
     <x:row r="73" spans="1:7">
       <x:c r="A73" s="0" t="s">
+        <x:v>228</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
         <x:v>229</x:v>
       </x:c>
-      <x:c r="B73" s="0" t="s">
+      <x:c r="C73" s="0" t="s">
         <x:v>230</x:v>
       </x:c>
-      <x:c r="C73" s="0" t="s">
+      <x:c r="D73" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E73" s="0" t="s">
         <x:v>231</x:v>
       </x:c>
-      <x:c r="D73" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E73" s="0" t="s">
-        <x:v>232</x:v>
-      </x:c>
       <x:c r="F73" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="G73" s="0" t="s">
         <x:v>13</x:v>
@@ -3008,22 +3005,22 @@
     </x:row>
     <x:row r="74" spans="1:7">
       <x:c r="A74" s="0" t="s">
+        <x:v>232</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
         <x:v>233</x:v>
       </x:c>
-      <x:c r="B74" s="0" t="s">
+      <x:c r="C74" s="0" t="s">
         <x:v>234</x:v>
       </x:c>
-      <x:c r="C74" s="0" t="s">
+      <x:c r="D74" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E74" s="0" t="s">
         <x:v>235</x:v>
       </x:c>
-      <x:c r="D74" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E74" s="0" t="s">
+      <x:c r="F74" s="0" t="s">
         <x:v>236</x:v>
-      </x:c>
-      <x:c r="F74" s="0" t="s">
-        <x:v>228</x:v>
       </x:c>
       <x:c r="G74" s="0" t="s">
         <x:v>133</x:v>
@@ -3031,22 +3028,22 @@
     </x:row>
     <x:row r="75" spans="1:7">
       <x:c r="A75" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
         <x:v>237</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="D75" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E75" s="0" t="s">
         <x:v>189</x:v>
       </x:c>
-      <x:c r="D75" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E75" s="0" t="s">
-        <x:v>190</x:v>
-      </x:c>
       <x:c r="F75" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G75" s="0" t="s">
         <x:v>133</x:v>
@@ -3069,7 +3066,7 @@
         <x:v>241</x:v>
       </x:c>
       <x:c r="F76" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G76" s="0" t="s">
         <x:v>242</x:v>
@@ -3092,7 +3089,7 @@
         <x:v>246</x:v>
       </x:c>
       <x:c r="F77" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G77" s="0" t="s">
         <x:v>146</x:v>
@@ -3115,30 +3112,30 @@
         <x:v>250</x:v>
       </x:c>
       <x:c r="F78" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G78" s="0" t="s">
         <x:v>251</x:v>
-      </x:c>
-      <x:c r="G78" s="0" t="s">
-        <x:v>252</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:7">
       <x:c r="A79" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
         <x:v>253</x:v>
       </x:c>
-      <x:c r="B79" s="0" t="s">
+      <x:c r="C79" s="0" t="s">
         <x:v>254</x:v>
       </x:c>
-      <x:c r="C79" s="0" t="s">
+      <x:c r="D79" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E79" s="0" t="s">
         <x:v>255</x:v>
       </x:c>
-      <x:c r="D79" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E79" s="0" t="s">
-        <x:v>256</x:v>
-      </x:c>
       <x:c r="F79" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G79" s="0" t="s">
         <x:v>151</x:v>
@@ -3146,45 +3143,45 @@
     </x:row>
     <x:row r="80" spans="1:7">
       <x:c r="A80" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
         <x:v>257</x:v>
       </x:c>
-      <x:c r="B80" s="0" t="s">
+      <x:c r="C80" s="0" t="s">
         <x:v>258</x:v>
       </x:c>
-      <x:c r="C80" s="0" t="s">
+      <x:c r="D80" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E80" s="0" t="s">
         <x:v>259</x:v>
       </x:c>
-      <x:c r="D80" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E80" s="0" t="s">
-        <x:v>260</x:v>
-      </x:c>
       <x:c r="F80" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G80" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:7">
       <x:c r="A81" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
         <x:v>261</x:v>
       </x:c>
-      <x:c r="B81" s="0" t="s">
+      <x:c r="C81" s="0" t="s">
         <x:v>262</x:v>
       </x:c>
-      <x:c r="C81" s="0" t="s">
+      <x:c r="D81" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E81" s="0" t="s">
         <x:v>263</x:v>
       </x:c>
-      <x:c r="D81" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E81" s="0" t="s">
-        <x:v>264</x:v>
-      </x:c>
       <x:c r="F81" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G81" s="0" t="s">
         <x:v>133</x:v>
@@ -3192,68 +3189,68 @@
     </x:row>
     <x:row r="82" spans="1:7">
       <x:c r="A82" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
         <x:v>265</x:v>
       </x:c>
-      <x:c r="B82" s="0" t="s">
+      <x:c r="C82" s="0" t="s">
         <x:v>266</x:v>
       </x:c>
-      <x:c r="C82" s="0" t="s">
+      <x:c r="D82" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E82" s="0" t="s">
         <x:v>267</x:v>
       </x:c>
-      <x:c r="D82" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E82" s="0" t="s">
+      <x:c r="F82" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G82" s="0" t="s">
         <x:v>268</x:v>
-      </x:c>
-      <x:c r="F82" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-      <x:c r="G82" s="0" t="s">
-        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:7">
       <x:c r="A83" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
         <x:v>270</x:v>
       </x:c>
-      <x:c r="B83" s="0" t="s">
+      <x:c r="C83" s="0" t="s">
         <x:v>271</x:v>
       </x:c>
-      <x:c r="C83" s="0" t="s">
+      <x:c r="D83" s="0" t="s">
         <x:v>272</x:v>
       </x:c>
-      <x:c r="D83" s="0" t="s">
+      <x:c r="E83" s="0" t="s">
         <x:v>273</x:v>
       </x:c>
-      <x:c r="E83" s="0" t="s">
-        <x:v>274</x:v>
-      </x:c>
       <x:c r="F83" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G83" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>268</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:7">
       <x:c r="A84" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
         <x:v>275</x:v>
       </x:c>
-      <x:c r="B84" s="0" t="s">
+      <x:c r="C84" s="0" t="s">
         <x:v>276</x:v>
       </x:c>
-      <x:c r="C84" s="0" t="s">
+      <x:c r="D84" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E84" s="0" t="s">
         <x:v>277</x:v>
       </x:c>
-      <x:c r="D84" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E84" s="0" t="s">
-        <x:v>278</x:v>
-      </x:c>
       <x:c r="F84" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G84" s="0" t="s">
         <x:v>133</x:v>
@@ -3261,45 +3258,45 @@
     </x:row>
     <x:row r="85" spans="1:7">
       <x:c r="A85" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
         <x:v>279</x:v>
       </x:c>
-      <x:c r="B85" s="0" t="s">
+      <x:c r="C85" s="0" t="s">
         <x:v>280</x:v>
       </x:c>
-      <x:c r="C85" s="0" t="s">
+      <x:c r="D85" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E85" s="0" t="s">
         <x:v>281</x:v>
       </x:c>
-      <x:c r="D85" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E85" s="0" t="s">
-        <x:v>282</x:v>
-      </x:c>
       <x:c r="F85" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G85" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:7">
       <x:c r="A86" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
         <x:v>283</x:v>
       </x:c>
-      <x:c r="B86" s="0" t="s">
+      <x:c r="C86" s="0" t="s">
         <x:v>284</x:v>
       </x:c>
-      <x:c r="C86" s="0" t="s">
+      <x:c r="D86" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E86" s="0" t="s">
         <x:v>285</x:v>
       </x:c>
-      <x:c r="D86" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E86" s="0" t="s">
-        <x:v>286</x:v>
-      </x:c>
       <x:c r="F86" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G86" s="0" t="s">
         <x:v>133</x:v>
@@ -3307,22 +3304,22 @@
     </x:row>
     <x:row r="87" spans="1:7">
       <x:c r="A87" s="0" t="s">
-        <x:v>283</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
         <x:v>287</x:v>
       </x:c>
-      <x:c r="C87" s="0" t="s">
-        <x:v>288</x:v>
-      </x:c>
       <x:c r="D87" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E87" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="F87" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G87" s="0" t="s">
         <x:v>133</x:v>
@@ -3333,10 +3330,10 @@
         <x:v>157</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
         <x:v>289</x:v>
-      </x:c>
-      <x:c r="C88" s="0" t="s">
-        <x:v>290</x:v>
       </x:c>
       <x:c r="D88" s="0" t="s">
         <x:v>10</x:v>
@@ -3345,7 +3342,7 @@
         <x:v>160</x:v>
       </x:c>
       <x:c r="F88" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G88" s="0" t="s">
         <x:v>13</x:v>
@@ -3353,301 +3350,301 @@
     </x:row>
     <x:row r="89" spans="1:7">
       <x:c r="A89" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
         <x:v>291</x:v>
       </x:c>
-      <x:c r="B89" s="0" t="s">
+      <x:c r="C89" s="0" t="s">
         <x:v>292</x:v>
       </x:c>
-      <x:c r="C89" s="0" t="s">
+      <x:c r="D89" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E89" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D89" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E89" s="0" t="s">
+      <x:c r="F89" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G89" s="0" t="s">
         <x:v>294</x:v>
-      </x:c>
-      <x:c r="F89" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-      <x:c r="G89" s="0" t="s">
-        <x:v>295</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:7">
       <x:c r="A90" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E90" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D90" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E90" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F90" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G90" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:7">
       <x:c r="A91" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E91" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="F91" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G91" s="0" t="s">
         <x:v>297</x:v>
-      </x:c>
-      <x:c r="C91" s="0" t="s">
-        <x:v>293</x:v>
-      </x:c>
-      <x:c r="D91" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E91" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
-      <x:c r="F91" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-      <x:c r="G91" s="0" t="s">
-        <x:v>298</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:7">
       <x:c r="A92" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E92" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="F92" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G92" s="0" t="s">
         <x:v>299</x:v>
-      </x:c>
-      <x:c r="C92" s="0" t="s">
-        <x:v>293</x:v>
-      </x:c>
-      <x:c r="D92" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E92" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
-      <x:c r="F92" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-      <x:c r="G92" s="0" t="s">
-        <x:v>300</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:7">
       <x:c r="A93" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E93" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D93" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E93" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F93" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G93" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:7">
       <x:c r="A94" s="0" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
         <x:v>302</x:v>
       </x:c>
-      <x:c r="B94" s="0" t="s">
+      <x:c r="C94" s="0" t="s">
         <x:v>303</x:v>
       </x:c>
-      <x:c r="C94" s="0" t="s">
+      <x:c r="D94" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E94" s="0" t="s">
         <x:v>304</x:v>
       </x:c>
-      <x:c r="D94" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E94" s="0" t="s">
-        <x:v>305</x:v>
-      </x:c>
       <x:c r="F94" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G94" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>108</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:7">
       <x:c r="A95" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E95" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="F95" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G95" s="0" t="s">
         <x:v>306</x:v>
-      </x:c>
-      <x:c r="C95" s="0" t="s">
-        <x:v>293</x:v>
-      </x:c>
-      <x:c r="D95" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E95" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
-      <x:c r="F95" s="0" t="s">
-        <x:v>251</x:v>
-      </x:c>
-      <x:c r="G95" s="0" t="s">
-        <x:v>307</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:7">
       <x:c r="A96" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E96" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D96" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E96" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F96" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G96" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:7">
       <x:c r="A97" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>309</x:v>
+        <x:v>308</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E97" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D97" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E97" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F97" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G97" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:7">
       <x:c r="A98" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E98" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D98" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E98" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F98" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G98" s="0" t="s">
-        <x:v>298</x:v>
+        <x:v>297</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:7">
       <x:c r="A99" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>310</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E99" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D99" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E99" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F99" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G99" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:7">
       <x:c r="A100" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E100" s="0" t="s">
         <x:v>293</x:v>
       </x:c>
-      <x:c r="D100" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E100" s="0" t="s">
-        <x:v>294</x:v>
-      </x:c>
       <x:c r="F100" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="G100" s="0" t="s">
-        <x:v>298</x:v>
+        <x:v>297</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:7">
       <x:c r="A101" s="0" t="s">
+        <x:v>312</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
         <x:v>313</x:v>
       </x:c>
-      <x:c r="B101" s="0" t="s">
+      <x:c r="C101" s="0" t="s">
         <x:v>314</x:v>
       </x:c>
-      <x:c r="C101" s="0" t="s">
+      <x:c r="D101" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E101" s="0" t="s">
         <x:v>315</x:v>
       </x:c>
-      <x:c r="D101" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E101" s="0" t="s">
-        <x:v>316</x:v>
-      </x:c>
       <x:c r="F101" s="0" t="s">
+        <x:v>236</x:v>
+      </x:c>
+      <x:c r="G101" s="0" t="s">
         <x:v>251</x:v>
-      </x:c>
-      <x:c r="G101" s="0" t="s">
-        <x:v>252</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>